<commit_message>
Tawarruq AppDataCheck Employement Details Auto Loan Offering Facility Details
</commit_message>
<xml_diff>
--- a/ULS_Jay/TestData/IjaraJSPaths.xlsx
+++ b/ULS_Jay/TestData/IjaraJSPaths.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="11610" windowHeight="8040" tabRatio="599" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="11610" windowHeight="8040" tabRatio="599" firstSheet="14" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Ijara_loginElements" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,14 @@
     <sheet name="_" sheetId="14" r:id="rId16"/>
     <sheet name="Al_ADEntry_CustomerDetails_610" sheetId="15" r:id="rId17"/>
     <sheet name="Al_ADEntryDocDetails_610" sheetId="16" r:id="rId18"/>
+    <sheet name="TA_ADC_EmploymentDetails" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="1528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="1807">
   <si>
     <t>Ijara_LoginFieldName</t>
   </si>
@@ -4197,9 +4198,6 @@
     <t>DeclaredDownPaymentAmount</t>
   </si>
   <si>
-    <t>document.querySelector('kub-prime-ccy[id="downPaymentAmount"]')</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -4365,9 +4363,6 @@
     <t>document.querySelector('digital-text-box[id="loanTenure"]').querySelector('input')</t>
   </si>
   <si>
-    <t>document.querySelector('kub-prime-ccy[id="downPaymentAmount"]').querySelector('p-inputnumber')</t>
-  </si>
-  <si>
     <t>ListView</t>
   </si>
   <si>
@@ -4615,6 +4610,849 @@
   </si>
   <si>
     <t>scrollUpCustomerDetails</t>
+  </si>
+  <si>
+    <t>Facility_info_Tab_AL</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-segment-button[id="seg8"]')</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="facilityTypeCode"] ')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="downPaymentAmount"]')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="downPaymentAmount"]').querySelector('p-inputnumber')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="downPaymentAmount"]').querySelector('ion-input')</t>
+  </si>
+  <si>
+    <t>DeclaredDownPaymentAmountTypeAL</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-radio-button[id="recStatus"]')</t>
+  </si>
+  <si>
+    <t>status_ToggleButton_NonEdi</t>
+  </si>
+  <si>
+    <t>EmploymentDetails_FieldName</t>
+  </si>
+  <si>
+    <t>SalariedEmpDetails_eyeBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelector('button[icon="pi pi-eye"]')</t>
+  </si>
+  <si>
+    <t>businessEmpDetails_eyeBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelectorAll('button[icon="pi pi-eye"]')[1]</t>
+  </si>
+  <si>
+    <t>companyFirmEmpDetails_eyeBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelectorAll('button[icon="pi pi-eye"]')[2]</t>
+  </si>
+  <si>
+    <t>pensionerEmpDetails_eyeBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelectorAll('button[icon="pi pi-eye"]')[3]</t>
+  </si>
+  <si>
+    <t>selfEmployed_eyeBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelectorAll('button[icon="pi pi-eye"]')[4]</t>
+  </si>
+  <si>
+    <t>EmpDetailsSectionNextPageBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[class="p-ripple p-element p-paginator-next p-paginator-element p-link"]')</t>
+  </si>
+  <si>
+    <t>selfEmployedProfessional_eyeBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelectorAll('button[icon="pi pi-eye"]')[0]</t>
+  </si>
+  <si>
+    <t>customerEmploymentBackBtn</t>
+  </si>
+  <si>
+    <t>primaryEmployment</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="isPrimaryEmployment"]')</t>
+  </si>
+  <si>
+    <t>primaryEmploymentLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="isPrimaryEmployment"] ion-label')</t>
+  </si>
+  <si>
+    <t>primaryEmploymentToggleBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="isPrimaryEmployment"] ion-toggle')</t>
+  </si>
+  <si>
+    <t>employmentPeriod</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentStatus"]')</t>
+  </si>
+  <si>
+    <t>employmentPeriodLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentStatus"] ion-label')</t>
+  </si>
+  <si>
+    <t>employmentPeriodDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentStatus"] ion-select')</t>
+  </si>
+  <si>
+    <t>natureOfEmployment</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentType"]')</t>
+  </si>
+  <si>
+    <t>natureOfEmploymentLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentType"] ion-label')</t>
+  </si>
+  <si>
+    <t>natureOfEmploymentDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentType"] ion-select')</t>
+  </si>
+  <si>
+    <t>companyType</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="companyType"]')</t>
+  </si>
+  <si>
+    <t>companyTypeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="companyType"] ion-label')</t>
+  </si>
+  <si>
+    <t>companyTypeDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="companyType"] ion-select')</t>
+  </si>
+  <si>
+    <t>profession</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="typeOfProfessionCode"]')</t>
+  </si>
+  <si>
+    <t>professionLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="typeOfProfessionCode"] ion-label')</t>
+  </si>
+  <si>
+    <t>professionDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="typeOfProfessionCode"] ion-select')</t>
+  </si>
+  <si>
+    <t>professionType</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="typeOfProfession"]')</t>
+  </si>
+  <si>
+    <t>professionTypeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="typeOfProfession"] ion-label')</t>
+  </si>
+  <si>
+    <t>professionTypeDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="typeOfProfession"] ion-select')</t>
+  </si>
+  <si>
+    <t>statutoryAuthority</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredStatutoryAuthority"]')</t>
+  </si>
+  <si>
+    <t>statutoryAuthorityLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredStatutoryAuthority"] ion-label')</t>
+  </si>
+  <si>
+    <t>statutoryAuthorityDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredStatutoryAuthority"] ion-select')</t>
+  </si>
+  <si>
+    <t>employerName</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="employerName"]')</t>
+  </si>
+  <si>
+    <t>employerNameLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="employerName"] ion-label')</t>
+  </si>
+  <si>
+    <t>employerNameDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerName"] ion-select')</t>
+  </si>
+  <si>
+    <t>employerNameOthers</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="employerName"]')</t>
+  </si>
+  <si>
+    <t>employerNameOthersLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="employerName"] ion-label')</t>
+  </si>
+  <si>
+    <t>employerNameOthersInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="employerName"] ion-input')</t>
+  </si>
+  <si>
+    <t>employeeID</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employeeNumber"]')</t>
+  </si>
+  <si>
+    <t>employeeIDLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employeeNumber"] ion-label')</t>
+  </si>
+  <si>
+    <t>employeeIDInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employeeNumber"] ion-input')</t>
+  </si>
+  <si>
+    <t>dateOfJoining</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dateOfJoining"]')</t>
+  </si>
+  <si>
+    <t>dateOfJoiningLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dateOfJoining"] label')</t>
+  </si>
+  <si>
+    <t>dateOfJoiningCalender</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dateOfJoining"] p-calendar')</t>
+  </si>
+  <si>
+    <t>employmentEndDate</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentEndDate"]')</t>
+  </si>
+  <si>
+    <t>employmentEndDateLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentEndDate"] label')</t>
+  </si>
+  <si>
+    <t>employmentEndDateCalender</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employmentEndDate"] p-calendar')</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="department"]')</t>
+  </si>
+  <si>
+    <t>departmentLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="department"] ion-label')</t>
+  </si>
+  <si>
+    <t>departmentDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="department"] ion-select')</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="designation"]')</t>
+  </si>
+  <si>
+    <t>designationLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="designation"] ion-label')</t>
+  </si>
+  <si>
+    <t>designationDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="designation"] ion-select')</t>
+  </si>
+  <si>
+    <t>employmentType</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="isMilitaryOrCivil"]')</t>
+  </si>
+  <si>
+    <t>employmentTypeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="isMilitaryOrCivil"] ion-label')</t>
+  </si>
+  <si>
+    <t>employmentTypeDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="isMilitaryOrCivil"] ion-select')</t>
+  </si>
+  <si>
+    <t>directManagerContactNbr</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="contactNumberExtension"]')</t>
+  </si>
+  <si>
+    <t>directManagerContactNbrLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="contactNumberExtension"] ion-label')</t>
+  </si>
+  <si>
+    <t>directManagerContactNbrInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="contactNumberExtension"] input')</t>
+  </si>
+  <si>
+    <t>directManagerTelephone</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="contactNumber"]')</t>
+  </si>
+  <si>
+    <t>directManagerTelephoneLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="contactNumber"] ion-label')</t>
+  </si>
+  <si>
+    <t>directManagerTelephoneInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="contactNumber"] input')</t>
+  </si>
+  <si>
+    <t>incomePaymode</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="incomePaymode"]')</t>
+  </si>
+  <si>
+    <t>incomePaymodeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="incomePaymode"] ion-label')</t>
+  </si>
+  <si>
+    <t>incomePaymodeDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="incomePaymode"] ion-select')</t>
+  </si>
+  <si>
+    <t>employerPhoneExtension</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneExtension"]')</t>
+  </si>
+  <si>
+    <t>employerPhoneExLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneExtension"] ion-label')</t>
+  </si>
+  <si>
+    <t>employerPhoneExInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneExtension"] input')</t>
+  </si>
+  <si>
+    <t>employerPhoneNbr</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneNumber"]')</t>
+  </si>
+  <si>
+    <t>employerPhoneNbrLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneNumber"] ion-label')</t>
+  </si>
+  <si>
+    <t>employerPhoneNbrInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneNumber"] input')</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField1"]')</t>
+  </si>
+  <si>
+    <t>stateLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField1"] ion-label')</t>
+  </si>
+  <si>
+    <t>stateDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField1"] ion-select')</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField2"]')</t>
+  </si>
+  <si>
+    <t>cityLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField2"] ion-label')</t>
+  </si>
+  <si>
+    <t>cityDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField2"] ion-select')</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField3"]')</t>
+  </si>
+  <si>
+    <t>pincodeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField3"] ion-label')</t>
+  </si>
+  <si>
+    <t>pincodeInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="dynamicChararterField3"] input')</t>
+  </si>
+  <si>
+    <t>totalExperience</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="totalExperience"]')</t>
+  </si>
+  <si>
+    <t>totalExperienceLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="totalExperience"] ion-label')</t>
+  </si>
+  <si>
+    <t>totalExperienceInput</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="sectorEconomy"]')</t>
+  </si>
+  <si>
+    <t>sectorLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="sectorEconomy"] ion-label')</t>
+  </si>
+  <si>
+    <t>sectorDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="sectorEconomy"] ion-select')</t>
+  </si>
+  <si>
+    <t>subSector</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="subSector"]')</t>
+  </si>
+  <si>
+    <t>subSectorLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="subSector"] ion-label')</t>
+  </si>
+  <si>
+    <t>subSectorDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="subSector"] ion-select')</t>
+  </si>
+  <si>
+    <t>noOfPartners</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="numberOfPartners"]')</t>
+  </si>
+  <si>
+    <t>noOfPartnersLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="numberOfPartners"] ion-label')</t>
+  </si>
+  <si>
+    <t>noOfPartnersInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="numberOfPartners"] input')</t>
+  </si>
+  <si>
+    <t>natureOfBusiness</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="businessActivity"]')</t>
+  </si>
+  <si>
+    <t>natureOfBusinessLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="businessActivity"] ion-label')</t>
+  </si>
+  <si>
+    <t>natureOfBusinessDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="businessActivity"] ion-select')</t>
+  </si>
+  <si>
+    <t>regBusinessName</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessName"]')</t>
+  </si>
+  <si>
+    <t>regBusinessNameLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessName"] ion-label')</t>
+  </si>
+  <si>
+    <t>regBusinessNameInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessName"] input')</t>
+  </si>
+  <si>
+    <t>regBusinessNbr</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessNumber"]')</t>
+  </si>
+  <si>
+    <t>regBusinessNbrLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessNumber"] ion-label')</t>
+  </si>
+  <si>
+    <t>regBusinessNbrInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessNumber"] input')</t>
+  </si>
+  <si>
+    <t>businessRegisteredDate</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessDate"]')</t>
+  </si>
+  <si>
+    <t>businessRegisteredDateLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessDate"] label')</t>
+  </si>
+  <si>
+    <t>businessRegisteredDateCalender</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="registeredBusinessDate"] p-calendar')</t>
+  </si>
+  <si>
+    <t>officePremisesType</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="officePremisesType"]')</t>
+  </si>
+  <si>
+    <t>officePremisesTypeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="officePremisesType"] ion-label')</t>
+  </si>
+  <si>
+    <t>officePremisesTypeDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="officePremisesType"] ion-select')</t>
+  </si>
+  <si>
+    <t>shareHolderPercent</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="shareholderPercentage"]')</t>
+  </si>
+  <si>
+    <t>shareHolderPercentLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="shareholderPercentage"] ion-label')</t>
+  </si>
+  <si>
+    <t>shareHolderPercentInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="shareholderPercentage"] ion-input')</t>
+  </si>
+  <si>
+    <t>numberOfEmployees</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="numberOfEmployees"]')</t>
+  </si>
+  <si>
+    <t>numberOfEmployeesLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="numberOfEmployees"] ion-label')</t>
+  </si>
+  <si>
+    <t>numberOfEmployeesInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="numberOfEmployees"] input')</t>
+  </si>
+  <si>
+    <t>experienceAtCurrentEmployment</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="yearsAtCurrentEmployment"]')</t>
+  </si>
+  <si>
+    <t>experienceAtCurrentEmploymentLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="yearsAtCurrentEmployment"] ion-label')</t>
+  </si>
+  <si>
+    <t>experienceAtCurrentEmploymentInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="yearsAtCurrentEmployment"] input')</t>
+  </si>
+  <si>
+    <t>directManagerName</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="managerName"]')</t>
+  </si>
+  <si>
+    <t>directManagerNameLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="managerName"] ion-label')</t>
+  </si>
+  <si>
+    <t>directManagerNameInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="managerName"] input')</t>
+  </si>
+  <si>
+    <t>employerCityCode</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneCityCode"]')</t>
+  </si>
+  <si>
+    <t>employerCityCodeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneCityCode"] ion-label')</t>
+  </si>
+  <si>
+    <t>employerCityCodeInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="employerPhoneCityCode"] input')</t>
+  </si>
+  <si>
+    <t>retirementAge</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="retirementAge"]')</t>
+  </si>
+  <si>
+    <t>retirementAgeLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="retirementAge"] ion-label')</t>
+  </si>
+  <si>
+    <t>retirementAgeInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="retirementAge"] input')</t>
+  </si>
+  <si>
+    <t>recordStatus</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="recStatus"]')</t>
+  </si>
+  <si>
+    <t>recordStatusLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="recStatus"] ion-label')</t>
+  </si>
+  <si>
+    <t>recordStatusToggleBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="recStatus"] ion-toggle')</t>
+  </si>
+  <si>
+    <t>remarksTextarea</t>
+  </si>
+  <si>
+    <t>document.querySelector('[id="remarks"] ion-textarea')</t>
+  </si>
+  <si>
+    <t>listview_SearchBtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelector('button[icon="pi pi-search"]')</t>
+  </si>
+  <si>
+    <t>listview_EmployerName</t>
+  </si>
+  <si>
+    <t>listview_EmploymentStatus</t>
+  </si>
+  <si>
+    <t>listview_EmpValues</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelectorAll('tr')[1]</t>
+  </si>
+  <si>
+    <t>searchbox_Input</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-arrow-left"]').parentElement.parentElement.parentElement.querySelector('p-paginator span[class*="p-paginator-current"]')</t>
+  </si>
+  <si>
+    <t>document.querySelectorAll('button[ng-reflect-icon="pi pi-search"]')[1]</t>
+  </si>
+  <si>
+    <t>searchbtn</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[ng-reflect-text="Go Back"]').parentElement.parentElement.nextElementSibling.querySelector('button')</t>
+  </si>
+  <si>
+    <t>CustomerSearchBtn</t>
+  </si>
+  <si>
+    <t>CustomerFinanceTab</t>
+  </si>
+  <si>
+    <t>document.querySelectorAll('input[type="text"]')[3]</t>
+  </si>
+  <si>
+    <t>searchInput</t>
+  </si>
+  <si>
+    <t>document.querySelectorAll('button[ng-reflect-text="Go Back"]')[0].parentElement.parentElement.nextElementSibling.querySelector('button')</t>
+  </si>
+  <si>
+    <t>searchbtnTA</t>
+  </si>
+  <si>
+    <t>document.querySelectorAll('button[ng-reflect-text="Go Back"]')[0].parentElement.parentElement.nextElementSibling.querySelector('input')</t>
+  </si>
+  <si>
+    <t>searchInputTA</t>
+  </si>
+  <si>
+    <t>document.querySelectorAll('button[ng-reflect-text="Go Back"]')[0].parentElement.parentElement.nextElementSibling.querySelector('[icon="pi pi-eye"]')</t>
+  </si>
+  <si>
+    <t>viewBtnTA</t>
   </si>
 </sst>
 </file>
@@ -5817,7 +6655,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6029,7 +6867,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -6508,8 +7346,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A166" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6544,10 +7382,10 @@
     </row>
     <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="24" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6624,10 +7462,10 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="B16" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -6664,10 +7502,10 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="B21" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -6888,10 +7726,10 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="B50" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -7029,10 +7867,10 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="B70" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -7463,137 +8301,137 @@
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="27" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.75">
       <c r="A136" s="24" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="B136" s="24" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.75">
       <c r="A137" s="24" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="B137" s="24" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15.75">
       <c r="A138" s="24" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="B138" s="24" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15.75">
       <c r="A139" s="24" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="B139" s="24" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15.75">
       <c r="A140" s="24" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="B140" s="24" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.75">
       <c r="A141" s="24" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="B141" s="24" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.75">
       <c r="A143" s="28" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75">
       <c r="A145" s="24" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B145" s="24" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15.75">
       <c r="A146" s="24" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="B146" s="24" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15.75">
       <c r="A147" s="24" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="B147" s="24" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.75">
       <c r="A148" s="24" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="B148" s="24" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.75">
       <c r="A149" s="24" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="B149" s="24" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15.75">
       <c r="A150" s="24" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="B150" s="24" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="28" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15.75">
       <c r="A154" s="24" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="B154" s="24" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15.75">
       <c r="A155" s="24" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="B155" s="24" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15.75">
       <c r="A156" s="24" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="B156" s="24" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15.75">
@@ -7622,77 +8460,77 @@
     </row>
     <row r="160" spans="1:2" ht="15.75">
       <c r="A160" s="24" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="B160" s="24" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="27" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15.75">
       <c r="A165" s="24" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="B165" s="24" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="C165" s="24"/>
     </row>
     <row r="166" spans="1:3" ht="15.75">
       <c r="A166" s="24" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="B166" s="24" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="C166" s="24"/>
     </row>
     <row r="167" spans="1:3" ht="15.75">
       <c r="A167" s="24" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="B167" s="24" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="C167" s="24"/>
     </row>
     <row r="168" spans="1:3" ht="15.75">
       <c r="A168" s="24" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="B168" s="24" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="C168" s="24"/>
     </row>
     <row r="169" spans="1:3" ht="15.75">
       <c r="A169" s="24" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="B169" s="24" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="C169" s="24"/>
     </row>
     <row r="170" spans="1:3" ht="15.75">
       <c r="A170" s="24" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="B170" s="24" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="C170" s="24"/>
     </row>
     <row r="171" spans="1:3" ht="15.75">
       <c r="A171" s="24" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="B171" s="24" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="C171" s="24"/>
     </row>
@@ -7701,28 +8539,28 @@
         <v>1340</v>
       </c>
       <c r="B172" s="24" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="15.75">
       <c r="A173" s="24" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="B173" s="24" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="15.75">
       <c r="A174" s="24" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B174" s="24" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="15.75">
       <c r="A175" s="24" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B175" s="24" t="s">
         <v>669</v>
@@ -7730,7 +8568,7 @@
     </row>
     <row r="176" spans="1:3" ht="15.75">
       <c r="A176" s="24" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B176" s="25" t="s">
         <v>671</v>
@@ -7741,25 +8579,25 @@
         <v>1340</v>
       </c>
       <c r="B177" s="24" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.75">
       <c r="A179" s="30" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15.75">
       <c r="A181" s="24" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="B181" s="24" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
     </row>
   </sheetData>
@@ -7773,8 +8611,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8004,13 +8842,1177 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B145"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="148.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="19" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>942</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B81" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B128" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>653</v>
+      </c>
+      <c r="B131" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B132" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B133" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B135" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>666</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B144" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B291"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A283" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A286" sqref="A286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8766,7 +10768,7 @@
     </row>
     <row r="117" spans="1:2" ht="15.75">
       <c r="A117" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="B117" s="24" t="s">
         <v>868</v>
@@ -9827,10 +11829,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9841,7 +11843,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="22" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>1</v>
@@ -9881,10 +11883,10 @@
     </row>
     <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="21" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>1427</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>1428</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75">
@@ -9897,7 +11899,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="21" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>746</v>
@@ -9913,7 +11915,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="21" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>748</v>
@@ -9929,10 +11931,10 @@
     </row>
     <row r="12" spans="1:2" ht="15.75">
       <c r="A12" s="21" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>1430</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>1431</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75">
@@ -9945,419 +11947,448 @@
     </row>
     <row r="14" spans="1:2" ht="15.75">
       <c r="A14" s="21" t="s">
-        <v>1377</v>
+        <v>1528</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1378</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75">
       <c r="A15" s="21" t="s">
-        <v>1433</v>
+        <v>1377</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>1434</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75">
       <c r="A16" s="21" t="s">
-        <v>1379</v>
+        <v>1432</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>1380</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75">
       <c r="A17" s="21" t="s">
-        <v>1436</v>
+        <v>1379</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>1435</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75">
       <c r="A18" s="21" t="s">
-        <v>1381</v>
+        <v>1435</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>1382</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75">
       <c r="A19" s="21" t="s">
-        <v>1438</v>
+        <v>1381</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>1437</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75">
       <c r="A20" s="21" t="s">
-        <v>1383</v>
+        <v>1437</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>1384</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75">
       <c r="A21" s="21" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75">
       <c r="A22" s="21" t="s">
-        <v>1439</v>
+        <v>1385</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>1444</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75">
       <c r="A23" s="21" t="s">
-        <v>1387</v>
+        <v>1533</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>1388</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75">
       <c r="A24" s="21" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>1440</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75">
       <c r="A25" s="21" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>1390</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75">
       <c r="A26" s="21" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75">
       <c r="A27" s="21" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75">
       <c r="A28" s="21" t="s">
-        <v>1393</v>
+        <v>1441</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>1394</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75">
       <c r="A29" s="21" t="s">
-        <v>1395</v>
+        <v>1390</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>1396</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75">
       <c r="A30" s="21" t="s">
-        <v>1397</v>
+        <v>1392</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>1398</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75">
       <c r="A31" s="21" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75">
       <c r="A32" s="21" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75">
       <c r="A33" s="21" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>712</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75">
       <c r="A34" s="21" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75">
       <c r="A35" s="21" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>1400</v>
+        <v>712</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75">
       <c r="A36" s="21" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>1396</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75">
       <c r="A37" s="21" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>1409</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75">
       <c r="A38" s="21" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>398</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75">
       <c r="A39" s="21" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75">
       <c r="A40" s="21" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>1414</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75">
       <c r="A41" s="21" t="s">
-        <v>1415</v>
+        <v>1410</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75">
       <c r="A42" s="21" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75">
       <c r="A43" s="21" t="s">
-        <v>1419</v>
+        <v>1414</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>1420</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75">
       <c r="A44" s="21" t="s">
-        <v>1421</v>
+        <v>1416</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>1422</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75">
       <c r="A45" s="21" t="s">
-        <v>1423</v>
+        <v>1418</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>1342</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75">
       <c r="A46" s="21" t="s">
-        <v>1424</v>
+        <v>1535</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>1344</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75">
       <c r="A47" s="21" t="s">
-        <v>1425</v>
+        <v>1420</v>
       </c>
       <c r="B47" s="21" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75">
+      <c r="A48" s="21" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75">
+      <c r="A49" s="21" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75">
+      <c r="A50" s="21" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B50" s="21" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75">
-      <c r="A49" s="23" t="s">
-        <v>1445</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75">
-      <c r="A51" s="24" t="s">
-        <v>1369</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>1446</v>
-      </c>
-    </row>
     <row r="52" spans="1:2" ht="15.75">
-      <c r="A52" s="24" t="s">
-        <v>1371</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>1447</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75">
-      <c r="A53" s="24" t="s">
-        <v>1449</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>1448</v>
+      <c r="A52" s="23" t="s">
+        <v>1443</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75">
       <c r="A54" s="24" t="s">
-        <v>1451</v>
+        <v>1369</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>1450</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75">
       <c r="A55" s="24" t="s">
-        <v>1453</v>
+        <v>1371</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>1452</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75">
       <c r="A56" s="24" t="s">
-        <v>1340</v>
+        <v>1447</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>1464</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75">
       <c r="A57" s="24" t="s">
-        <v>1458</v>
+        <v>1449</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>1457</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75">
       <c r="A58" s="24" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>1459</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75">
       <c r="A59" s="24" t="s">
-        <v>1454</v>
+        <v>1340</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>669</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75">
       <c r="A60" s="24" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B60" s="24" t="s">
         <v>1455</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75">
       <c r="A61" s="24" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75">
+      <c r="A62" s="24" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75">
+      <c r="A63" s="24" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75">
+      <c r="A64" s="24" t="s">
         <v>1340</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B64" s="24" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75">
+      <c r="A66" s="26" t="s">
         <v>1460</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75">
-      <c r="A63" s="26" t="s">
-        <v>1462</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="15.75">
-      <c r="A65" s="24" t="s">
-        <v>1463</v>
-      </c>
-      <c r="B65" s="24" t="s">
+    <row r="68" spans="1:2" ht="15.75">
+      <c r="A68" s="24" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="15.75">
-      <c r="A68" s="24"/>
-    </row>
-    <row r="70" spans="1:2" ht="15.75">
-      <c r="A70" s="24"/>
-      <c r="B70" s="24"/>
+      <c r="B68" s="24" t="s">
+        <v>1459</v>
+      </c>
     </row>
     <row r="71" spans="1:2" ht="15.75">
-      <c r="A71" s="24"/>
-      <c r="B71" s="24"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.75">
-      <c r="A72" s="24"/>
-      <c r="B72" s="24"/>
+      <c r="A71" s="21" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>1527</v>
+      </c>
     </row>
     <row r="73" spans="1:2" ht="15.75">
       <c r="A73" s="24"/>
       <c r="B73" s="24"/>
     </row>
+    <row r="74" spans="1:2" ht="15.75">
+      <c r="A74" s="24"/>
+      <c r="B74" s="24"/>
+    </row>
     <row r="75" spans="1:2" ht="15.75">
       <c r="A75" s="24"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.75">
-      <c r="A77" s="24"/>
-      <c r="B77" s="24"/>
+      <c r="B75" s="24"/>
+    </row>
+    <row r="76" spans="1:2" ht="15.75">
+      <c r="A76" s="24"/>
+      <c r="B76" s="24"/>
     </row>
     <row r="78" spans="1:2" ht="15.75">
       <c r="A78" s="24"/>
-      <c r="B78" s="24"/>
-    </row>
-    <row r="79" spans="1:2" ht="15.75">
-      <c r="A79" s="24"/>
-      <c r="B79" s="24"/>
     </row>
     <row r="80" spans="1:2" ht="15.75">
       <c r="A80" s="24"/>
       <c r="B80" s="24"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.75">
+      <c r="A81" s="24"/>
+      <c r="B81" s="24"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.75">
+      <c r="A82" s="24"/>
+      <c r="B82" s="24"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.75">
+      <c r="A83" s="24"/>
+      <c r="B83" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11633,8 +13664,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
committ : personal loan new app customer details
</commit_message>
<xml_diff>
--- a/ULS_Jay/TestData/IjaraJSPaths.xlsx
+++ b/ULS_Jay/TestData/IjaraJSPaths.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="11610" windowHeight="8040" tabRatio="599" firstSheet="14" activeTab="18"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="11610" windowHeight="8040" tabRatio="599" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Ijara_loginElements" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="Al_ADEntry_CustomerDetails_610" sheetId="15" r:id="rId17"/>
     <sheet name="Al_ADEntryDocDetails_610" sheetId="16" r:id="rId18"/>
     <sheet name="TA_ADC_EmploymentDetails" sheetId="19" r:id="rId19"/>
+    <sheet name="PL_NewApp_CustomerDetails_610" sheetId="20" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="1807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="1861">
   <si>
     <t>Ijara_LoginFieldName</t>
   </si>
@@ -5431,9 +5432,6 @@
     <t>CustomerFinanceTab</t>
   </si>
   <si>
-    <t>document.querySelectorAll('input[type="text"]')[3]</t>
-  </si>
-  <si>
     <t>searchInput</t>
   </si>
   <si>
@@ -5453,6 +5451,171 @@
   </si>
   <si>
     <t>viewBtnTA</t>
+  </si>
+  <si>
+    <t>PL_NewApp_CustomerDetails_FieldName</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="Customer Type.TOOLTIP"]')</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="Customer Type.TOOLTIP"]').nextElementSibling</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="CIF ID"]')</t>
+  </si>
+  <si>
+    <t>CifID</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="CIF ID"]').querySelector('input')</t>
+  </si>
+  <si>
+    <t>CifIDTextBox</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Application Number"]').querySelector('input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Application Number"]')</t>
+  </si>
+  <si>
+    <t>ApplicationNumber</t>
+  </si>
+  <si>
+    <t>ApplicationNumberText</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="ID Type.TOOLTIP"]').nextElementSibling</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="ID Type.TOOLTIP"]')</t>
+  </si>
+  <si>
+    <t>IDType</t>
+  </si>
+  <si>
+    <t>IDTypeDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="ID Number"]').querySelector('input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="ID Number"]')</t>
+  </si>
+  <si>
+    <t>IDNumber</t>
+  </si>
+  <si>
+    <t>IDNumberText</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Mobile Number"]').querySelector('input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Mobile Number"]')</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>MobileNumberText</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-prime-date[ng-reflect-title="Date of Birth"]')</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Email ID"]').querySelector('input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Email ID"]')</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>EmailIDText</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-prime-date[ng-reflect-title="Date of Birth"]').querySelector('input')</t>
+  </si>
+  <si>
+    <t>DOBInput</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[ptooltip="Search"]')</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[ptooltip="Clear"]')</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Customer Name"]').querySelector('input')</t>
+  </si>
+  <si>
+    <t>CustomerNameDropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Customer Name"]')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Mobile Number"]').querySelector('ion-input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="CIF ID"]').querySelector('ion-input')</t>
+  </si>
+  <si>
+    <t>IDTypeSelect</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="ID Number"]').querySelector('ion-input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Application Number"]').querySelector('ion-input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Customer Name"]').querySelector('ion-input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-prime-date[ng-reflect-title="Date of Birth"]').querySelector('p-calendar')</t>
+  </si>
+  <si>
+    <t>DOBCalendar</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[ng-reflect-title="Email ID"]').querySelector('ion-input')</t>
+  </si>
+  <si>
+    <t>CreateNewRequest</t>
+  </si>
+  <si>
+    <t>document.querySelectorAll('[class="p-element p-button-info p-button-sm w-90 m-2 pull-right p-button p-component"]')[2]</t>
+  </si>
+  <si>
+    <t>CifIDText</t>
+  </si>
+  <si>
+    <t>ApplicationNumberTex</t>
+  </si>
+  <si>
+    <t>CustomerNametext</t>
+  </si>
+  <si>
+    <t>IDNumberTex</t>
+  </si>
+  <si>
+    <t>MobileNumberTex</t>
+  </si>
+  <si>
+    <t>EmailIDTex</t>
   </si>
 </sst>
 </file>
@@ -7346,8 +7509,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8846,8 +9009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9954,26 +10117,26 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B139" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B140" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B141" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -9994,10 +10157,10 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B145" t="s">
-        <v>1799</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -11826,6 +11989,292 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="91.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="11" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75">
+      <c r="A6" s="24" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>691</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75">
+      <c r="A34" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C34" s="24"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet17"/>

</xml_diff>